<commit_message>
Align parameter for PKIX.27
</commit_message>
<xml_diff>
--- a/conformancelib/testdata/PIV-I_Carillon_Cards.xlsx
+++ b/conformancelib/testdata/PIV-I_Carillon_Cards.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bob.fontana\Documents\GitRepos\piv-conformance\conformancelib\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5CB0C5EA-C31D-4D7A-9513-0CB6B026A5C2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06896881-B63B-433F-9E0B-257DA8A6736B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1215" yWindow="960" windowWidth="28410" windowHeight="14550" tabRatio="500" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1305" windowWidth="28410" windowHeight="14550" tabRatio="500" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SP 800-85B Reference" sheetId="1" r:id="rId1"/>
@@ -4069,7 +4069,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
@@ -4267,12 +4267,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -8360,8 +8354,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:F464"/>
   <sheetViews>
-    <sheetView topLeftCell="A364" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C372" sqref="C372"/>
+    <sheetView topLeftCell="A370" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="D370" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
@@ -19460,9 +19454,7 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:IV29"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
   <cols>
@@ -19976,15 +19968,10 @@
       <c r="D13" s="6" t="s">
         <v>1023</v>
       </c>
-      <c r="E13" s="52" t="s">
-        <v>1078</v>
-      </c>
       <c r="F13" s="6" t="s">
         <v>759</v>
       </c>
-      <c r="G13" s="49" t="s">
-        <v>1227</v>
-      </c>
+      <c r="G13" s="49"/>
     </row>
     <row r="14" spans="1:256" ht="31.5" customHeight="1">
       <c r="A14" s="6" t="s">
@@ -21503,39 +21490,43 @@
       <c r="IU27" s="31"/>
       <c r="IV27" s="31"/>
     </row>
-    <row r="28" spans="1:256" ht="60">
-      <c r="A28" s="67" t="s">
+    <row r="28" spans="1:256" ht="63">
+      <c r="A28" s="6" t="s">
         <v>1254</v>
       </c>
-      <c r="B28" s="67" t="s">
+      <c r="B28" s="6" t="s">
         <v>1001</v>
       </c>
-      <c r="C28" s="67" t="s">
+      <c r="C28" s="6" t="s">
         <v>1255</v>
       </c>
-      <c r="D28" s="68" t="s">
+      <c r="D28" s="6" t="s">
         <v>586</v>
       </c>
-      <c r="E28" s="67"/>
-      <c r="F28" s="67"/>
-      <c r="G28" s="67"/>
-    </row>
-    <row r="29" spans="1:256" ht="30">
-      <c r="A29" s="53" t="s">
+      <c r="E28" s="6" t="s">
+        <v>1078</v>
+      </c>
+      <c r="F28" s="6"/>
+      <c r="G28" s="49" t="s">
+        <v>1227</v>
+      </c>
+    </row>
+    <row r="29" spans="1:256" ht="31.5">
+      <c r="A29" s="6" t="s">
         <v>1256</v>
       </c>
-      <c r="B29" s="67" t="s">
+      <c r="B29" s="6" t="s">
         <v>1001</v>
       </c>
-      <c r="C29" s="60" t="s">
+      <c r="C29" s="6" t="s">
         <v>1257</v>
       </c>
-      <c r="D29" s="55" t="s">
+      <c r="D29" s="6" t="s">
         <v>588</v>
       </c>
-      <c r="E29" s="67"/>
-      <c r="F29" s="67"/>
-      <c r="G29" s="67"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>